<commit_message>
newest updates without the image ocr recognition
</commit_message>
<xml_diff>
--- a/app/uploads/tt (1).xlsx
+++ b/app/uploads/tt (1).xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
   <si>
     <t xml:space="preserve">Monday</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t xml:space="preserve">agile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdl</t>
   </si>
   <si>
     <t xml:space="preserve">13:00 to 14:00</t>
@@ -260,10 +263,10 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1"/>
@@ -335,10 +338,13 @@
       <c r="E4" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="F4" s="0" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>12</v>
@@ -348,12 +354,12 @@
         <v>12</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>8</v>

</xml_diff>